<commit_message>
order list원본과 sales list 원본을 넣어둠
</commit_message>
<xml_diff>
--- a/data/SalesList.xlsx
+++ b/data/SalesList.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Clients" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Clients" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Payment" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Delivery" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="Log" sheetId="5" state="visible" r:id="rId5"/>
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z1"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,132 +442,164 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>관리번호</t>
+          <t>업체명</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>업체명</t>
+          <t>사업자번호</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>모델명</t>
+          <t>대표자</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Description</t>
+          <t>전화번호</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>수량</t>
+          <t>이메일</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>단가</t>
+          <t>주소</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>환율</t>
+          <t>특이사항</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>세율(%)</t>
+          <t>운송방법</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>공급가액</t>
+          <t>운송계정</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>세액</t>
+          <t>국가</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>합계금액</t>
+          <t>통화</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>기수금액</t>
+          <t>담당자</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>미수금액</t>
+          <t>수출허가구분</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
-          <t>견적일</t>
+          <t>수출허가번호</t>
         </is>
       </c>
       <c r="O1" s="1" t="inlineStr">
         <is>
-          <t>수주일</t>
+          <t>수출허가만료일</t>
         </is>
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>출고예정일</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>출고일</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>선적일</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>입금완료일</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>세금계산서발행일</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>계산서번호</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>수출신고번호</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>수출신고필증경로</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Status</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>비고</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>주문요청사항</t>
+          <t>사업자등록증경로</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>콕스</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>010-2314-1234</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>sue@coxcamera.com</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>디지털로 242</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ㅁㅇㄴㄻㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>DHL</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>콕</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>KR</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>KRW</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>하수민</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>해당 없음</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>해당 없음</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>2025-12-31</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>//cox_biz/business/SalesManager/attachments\사업자등록증\사업자등록증_콕스__251209.png</t>
         </is>
       </c>
     </row>
@@ -582,7 +614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:AD3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,47 +625,340 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>관리번호</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>업체명</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>사업자번호</t>
-        </is>
-      </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>대표자</t>
+          <t>모델명</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>전화번호</t>
+          <t>Description</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>이메일</t>
+          <t>수량</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>주소</t>
+          <t>단가</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>특이사항</t>
+          <t>환율</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>운송방법</t>
+          <t>세율(%)</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>운송계정</t>
+          <t>공급가액</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>세액</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>합계금액</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>기수금액</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>미수금액</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>견적일</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>수주일</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>출고예정일</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>출고일</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>선적일</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>입금완료일</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>세금계산서발행일</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>계산서번호</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>수출신고번호</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>수출신고필증경로</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>비고</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>주문요청사항</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>구분</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="inlineStr">
+        <is>
+          <t>프로젝트명</t>
+        </is>
+      </c>
+      <c r="AC1" s="1" t="inlineStr">
+        <is>
+          <t>통화</t>
+        </is>
+      </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>품목명</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>QT-251209-001</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>콕스</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ㄴㅇㄻㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="E2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="G2" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="J2" t="n">
+        <v>100</v>
+      </c>
+      <c r="K2" t="n">
+        <v>1100</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>1100</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>2025-12-09</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>견적</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>ㄻㄴㅇㄻㄹㅁㄴ</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr"/>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>내수</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄻㄴㅇ</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>KRW</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>ㅇㄹㅁㄴㅇㄹ</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>QT-251209-001</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>콕스</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ㅇㄻㄴ</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ㅇㄻㄴㅇㄹ</t>
+        </is>
+      </c>
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1200</v>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="n">
+        <v>10</v>
+      </c>
+      <c r="I3" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J3" t="n">
+        <v>120</v>
+      </c>
+      <c r="K3" t="n">
+        <v>1320</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>1320</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>2025-12-09</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>견적</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>ㄻㄴㅇㄻㄹㅁㄴ</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr"/>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>내수</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄻㄴㅇ</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>KRW</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>ㅁㄴㅇㄻ</t>
         </is>
       </c>
     </row>
@@ -755,7 +1080,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -782,6 +1107,50 @@
       <c r="D1" s="1" t="inlineStr">
         <is>
           <t>상세내용</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2025-12-09 15:57:24</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sue</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>업체 등록</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>업체명: 콕스</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2025-12-09 15:57:46</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sue</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>견적 등록</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>번호 [QT-251209-001] / 업체 [콕스]</t>
         </is>
       </c>
     </row>

</xml_diff>